<commit_message>
finalize use case points and update class diagram
</commit_message>
<xml_diff>
--- a/use-case-points.xlsx
+++ b/use-case-points.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\University\Desenvolvimento de Software I\desenvolvimento-de-software-I\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D283A7ED-D20E-48EA-8A86-D53738EEBB29}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17344592-41C2-4B8E-8F3C-ED79E1618854}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -683,56 +683,56 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1016,8 +1016,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:G73"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A49" zoomScale="153" zoomScaleNormal="153" workbookViewId="0">
-      <selection activeCell="B56" sqref="B56:C56"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="153" zoomScaleNormal="153" workbookViewId="0">
+      <selection activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1032,13 +1032,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="18.75" x14ac:dyDescent="0.2">
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="38"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="31"/>
     </row>
     <row r="4" spans="2:7" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="19" t="s">
@@ -1128,12 +1128,12 @@
       </c>
     </row>
     <row r="10" spans="2:7" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="31" t="s">
+      <c r="B10" s="34" t="s">
         <v>79</v>
       </c>
-      <c r="C10" s="32"/>
-      <c r="D10" s="32"/>
-      <c r="E10" s="32"/>
+      <c r="C10" s="35"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="35"/>
       <c r="F10" s="7">
         <f>SUM(F7:F9)</f>
         <v>7</v>
@@ -1174,10 +1174,12 @@
       <c r="D15" s="6">
         <v>5</v>
       </c>
-      <c r="E15" s="6"/>
+      <c r="E15" s="6">
+        <v>5</v>
+      </c>
       <c r="F15" s="7">
         <f>D15*E15</f>
-        <v>0</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.2">
@@ -1190,10 +1192,12 @@
       <c r="D16" s="16">
         <v>10</v>
       </c>
-      <c r="E16" s="16"/>
+      <c r="E16" s="16">
+        <v>2</v>
+      </c>
       <c r="F16" s="17">
         <f t="shared" ref="F16:F17" si="1">D16*E16</f>
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.2">
@@ -1206,22 +1210,24 @@
       <c r="D17" s="26">
         <v>15</v>
       </c>
-      <c r="E17" s="26"/>
+      <c r="E17" s="26">
+        <v>0</v>
+      </c>
       <c r="F17" s="23">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B18" s="31" t="s">
+      <c r="B18" s="34" t="s">
         <v>80</v>
       </c>
-      <c r="C18" s="32"/>
-      <c r="D18" s="32"/>
-      <c r="E18" s="32"/>
+      <c r="C18" s="35"/>
+      <c r="D18" s="35"/>
+      <c r="E18" s="35"/>
       <c r="F18" s="7">
         <f>SUM(F15:F17)</f>
-        <v>0</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -1259,7 +1265,9 @@
       <c r="D23" s="6">
         <v>2</v>
       </c>
-      <c r="E23" s="6"/>
+      <c r="E23" s="6">
+        <v>0</v>
+      </c>
       <c r="F23" s="7">
         <f>D23*E23</f>
         <v>0</v>
@@ -1293,10 +1301,12 @@
       <c r="D25" s="6">
         <v>1</v>
       </c>
-      <c r="E25" s="6"/>
+      <c r="E25" s="6">
+        <v>5</v>
+      </c>
       <c r="F25" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.2">
@@ -1309,10 +1319,12 @@
       <c r="D26" s="6">
         <v>1</v>
       </c>
-      <c r="E26" s="6"/>
+      <c r="E26" s="6">
+        <v>2</v>
+      </c>
       <c r="F26" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.2">
@@ -1325,10 +1337,12 @@
       <c r="D27" s="16">
         <v>1</v>
       </c>
-      <c r="E27" s="16"/>
+      <c r="E27" s="16">
+        <v>1</v>
+      </c>
       <c r="F27" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.2">
@@ -1341,10 +1355,12 @@
       <c r="D28" s="6">
         <v>0.5</v>
       </c>
-      <c r="E28" s="6"/>
+      <c r="E28" s="6">
+        <v>5</v>
+      </c>
       <c r="F28" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.2">
@@ -1357,10 +1373,12 @@
       <c r="D29" s="6">
         <v>0.5</v>
       </c>
-      <c r="E29" s="6"/>
+      <c r="E29" s="6">
+        <v>5</v>
+      </c>
       <c r="F29" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.2">
@@ -1373,7 +1391,9 @@
       <c r="D30" s="16">
         <v>2</v>
       </c>
-      <c r="E30" s="16"/>
+      <c r="E30" s="16">
+        <v>0</v>
+      </c>
       <c r="F30" s="7">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1389,10 +1409,12 @@
       <c r="D31" s="6">
         <v>1</v>
       </c>
-      <c r="E31" s="6"/>
+      <c r="E31" s="6">
+        <v>4</v>
+      </c>
       <c r="F31" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.2">
@@ -1405,10 +1427,12 @@
       <c r="D32" s="6">
         <v>1</v>
       </c>
-      <c r="E32" s="6"/>
+      <c r="E32" s="6">
+        <v>4</v>
+      </c>
       <c r="F32" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.2">
@@ -1421,10 +1445,12 @@
       <c r="D33" s="16">
         <v>1</v>
       </c>
-      <c r="E33" s="16"/>
+      <c r="E33" s="16">
+        <v>5</v>
+      </c>
       <c r="F33" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.2">
@@ -1437,10 +1463,12 @@
       <c r="D34" s="6">
         <v>1</v>
       </c>
-      <c r="E34" s="6"/>
+      <c r="E34" s="6">
+        <v>4</v>
+      </c>
       <c r="F34" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.2">
@@ -1453,34 +1481,36 @@
       <c r="D35" s="26">
         <v>1</v>
       </c>
-      <c r="E35" s="26"/>
+      <c r="E35" s="26">
+        <v>1</v>
+      </c>
       <c r="F35" s="23">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B36" s="31" t="s">
+      <c r="B36" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="C36" s="32"/>
-      <c r="D36" s="32"/>
-      <c r="E36" s="32"/>
+      <c r="C36" s="35"/>
+      <c r="D36" s="35"/>
+      <c r="E36" s="35"/>
       <c r="F36" s="7">
         <f>SUM(F23:F35)</f>
-        <v>4</v>
+        <v>35</v>
       </c>
     </row>
     <row r="37" spans="2:6" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B37" s="39" t="s">
+      <c r="B37" s="32" t="s">
         <v>81</v>
       </c>
-      <c r="C37" s="40"/>
-      <c r="D37" s="40"/>
-      <c r="E37" s="40"/>
+      <c r="C37" s="33"/>
+      <c r="D37" s="33"/>
+      <c r="E37" s="33"/>
       <c r="F37" s="7">
         <f>0.6+(0.01*F36)</f>
-        <v>0.64</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.2">
@@ -1518,10 +1548,12 @@
       <c r="D42" s="6">
         <v>1.5</v>
       </c>
-      <c r="E42" s="6"/>
+      <c r="E42" s="6">
+        <v>3</v>
+      </c>
       <c r="F42" s="7">
         <f>D42*E42</f>
-        <v>0</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.2">
@@ -1534,7 +1566,9 @@
       <c r="D43" s="16">
         <v>0.5</v>
       </c>
-      <c r="E43" s="16"/>
+      <c r="E43" s="16">
+        <v>0</v>
+      </c>
       <c r="F43" s="7">
         <f t="shared" ref="F43:F49" si="3">D43*E43</f>
         <v>0</v>
@@ -1550,10 +1584,12 @@
       <c r="D44" s="6">
         <v>1</v>
       </c>
-      <c r="E44" s="6"/>
+      <c r="E44" s="6">
+        <v>4</v>
+      </c>
       <c r="F44" s="7">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="45" spans="2:6" x14ac:dyDescent="0.2">
@@ -1566,10 +1602,12 @@
       <c r="D45" s="6">
         <v>0.5</v>
       </c>
-      <c r="E45" s="6"/>
+      <c r="E45" s="6">
+        <v>2</v>
+      </c>
       <c r="F45" s="7">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="2:6" x14ac:dyDescent="0.2">
@@ -1582,10 +1620,12 @@
       <c r="D46" s="16">
         <v>1</v>
       </c>
-      <c r="E46" s="16"/>
+      <c r="E46" s="16">
+        <v>5</v>
+      </c>
       <c r="F46" s="7">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="47" spans="2:6" x14ac:dyDescent="0.2">
@@ -1598,10 +1638,12 @@
       <c r="D47" s="6">
         <v>2</v>
       </c>
-      <c r="E47" s="6"/>
+      <c r="E47" s="6">
+        <v>5</v>
+      </c>
       <c r="F47" s="7">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="48" spans="2:6" x14ac:dyDescent="0.2">
@@ -1614,10 +1656,12 @@
       <c r="D48" s="6">
         <v>-1</v>
       </c>
-      <c r="E48" s="6"/>
+      <c r="E48" s="6">
+        <v>3</v>
+      </c>
       <c r="F48" s="7">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="49" spans="2:6" x14ac:dyDescent="0.2">
@@ -1630,190 +1674,192 @@
       <c r="D49" s="6">
         <v>-1.5</v>
       </c>
-      <c r="E49" s="6"/>
+      <c r="E49" s="6">
+        <v>5</v>
+      </c>
       <c r="F49" s="7">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>-7.5</v>
       </c>
     </row>
     <row r="50" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B50" s="39" t="s">
+      <c r="B50" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="C50" s="40"/>
-      <c r="D50" s="40"/>
-      <c r="E50" s="41"/>
+      <c r="C50" s="33"/>
+      <c r="D50" s="33"/>
+      <c r="E50" s="36"/>
       <c r="F50" s="12">
         <f>SUM(F42:F49)</f>
-        <v>0</v>
+        <v>14</v>
       </c>
     </row>
     <row r="51" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B51" s="42" t="s">
+      <c r="B51" s="37" t="s">
         <v>75</v>
       </c>
-      <c r="C51" s="42"/>
-      <c r="D51" s="42"/>
-      <c r="E51" s="42"/>
+      <c r="C51" s="37"/>
+      <c r="D51" s="37"/>
+      <c r="E51" s="37"/>
       <c r="F51" s="12">
         <f>1.4+(-0.03*F50)</f>
-        <v>1.4</v>
+        <v>0.98</v>
       </c>
     </row>
     <row r="53" spans="2:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B53" s="30" t="s">
+      <c r="B53" s="44" t="s">
         <v>90</v>
       </c>
-      <c r="C53" s="30"/>
+      <c r="C53" s="44"/>
       <c r="D53" s="13" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="54" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B54" s="43" t="s">
+      <c r="B54" s="38" t="s">
         <v>79</v>
       </c>
-      <c r="C54" s="44"/>
+      <c r="C54" s="39"/>
       <c r="D54" s="23">
         <f>F10</f>
         <v>7</v>
       </c>
     </row>
     <row r="55" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B55" s="43" t="s">
+      <c r="B55" s="38" t="s">
         <v>80</v>
       </c>
-      <c r="C55" s="44"/>
+      <c r="C55" s="39"/>
       <c r="D55" s="23">
         <f>F18</f>
-        <v>0</v>
+        <v>45</v>
       </c>
     </row>
     <row r="56" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B56" s="28" t="s">
+      <c r="B56" s="40" t="s">
         <v>81</v>
       </c>
-      <c r="C56" s="29"/>
+      <c r="C56" s="41"/>
       <c r="D56" s="7">
         <f>F37</f>
-        <v>0.64</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="57" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B57" s="43" t="s">
+      <c r="B57" s="38" t="s">
         <v>82</v>
       </c>
-      <c r="C57" s="44"/>
+      <c r="C57" s="39"/>
       <c r="D57" s="23">
         <f>F51</f>
-        <v>1.4</v>
+        <v>0.98</v>
       </c>
     </row>
     <row r="58" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B58" s="28" t="s">
+      <c r="B58" s="40" t="s">
         <v>78</v>
       </c>
-      <c r="C58" s="29"/>
+      <c r="C58" s="41"/>
       <c r="D58" s="27">
         <f xml:space="preserve"> (D54+D55)*D56*D57</f>
-        <v>6.2720000000000002</v>
+        <v>48.411999999999999</v>
       </c>
     </row>
     <row r="59" spans="2:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B59" s="33" t="s">
+      <c r="B59" s="42" t="s">
         <v>93</v>
       </c>
-      <c r="C59" s="34"/>
+      <c r="C59" s="43"/>
       <c r="D59" s="17">
         <f>D58*20</f>
-        <v>125.44</v>
+        <v>968.24</v>
       </c>
     </row>
     <row r="60" spans="2:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B60" s="28" t="s">
+      <c r="B60" s="40" t="s">
         <v>77</v>
       </c>
-      <c r="C60" s="29"/>
+      <c r="C60" s="41"/>
       <c r="D60" s="7">
         <v>3</v>
       </c>
     </row>
     <row r="61" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B61" s="33" t="s">
+      <c r="B61" s="42" t="s">
         <v>83</v>
       </c>
-      <c r="C61" s="34"/>
+      <c r="C61" s="43"/>
       <c r="D61" s="17">
         <f>D59/D60</f>
-        <v>41.813333333333333</v>
+        <v>322.74666666666667</v>
       </c>
     </row>
     <row r="62" spans="2:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B62" s="28" t="s">
+      <c r="B62" s="40" t="s">
         <v>85</v>
       </c>
-      <c r="C62" s="29"/>
+      <c r="C62" s="41"/>
       <c r="D62" s="7">
         <v>5</v>
       </c>
     </row>
     <row r="63" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B63" s="33" t="s">
+      <c r="B63" s="42" t="s">
         <v>86</v>
       </c>
-      <c r="C63" s="34"/>
+      <c r="C63" s="43"/>
       <c r="D63" s="17">
         <f>D61/D62</f>
-        <v>8.3626666666666658</v>
+        <v>64.549333333333337</v>
       </c>
     </row>
     <row r="64" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B64" s="28" t="s">
+      <c r="B64" s="40" t="s">
         <v>84</v>
       </c>
-      <c r="C64" s="29"/>
+      <c r="C64" s="41"/>
       <c r="D64" s="7">
         <f>D62*4</f>
         <v>20</v>
       </c>
     </row>
     <row r="65" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B65" s="33" t="s">
+      <c r="B65" s="42" t="s">
         <v>91</v>
       </c>
-      <c r="C65" s="34"/>
+      <c r="C65" s="43"/>
       <c r="D65" s="17">
         <f>D61/D64</f>
-        <v>2.0906666666666665</v>
+        <v>16.137333333333334</v>
       </c>
     </row>
     <row r="66" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B66" s="28" t="s">
+      <c r="B66" s="40" t="s">
         <v>87</v>
       </c>
-      <c r="C66" s="29"/>
+      <c r="C66" s="41"/>
       <c r="D66" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="67" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B67" s="33" t="s">
+      <c r="B67" s="42" t="s">
         <v>88</v>
       </c>
-      <c r="C67" s="34"/>
+      <c r="C67" s="43"/>
       <c r="D67" s="17">
         <f>D63+D66</f>
-        <v>9.3626666666666658</v>
+        <v>65.549333333333337</v>
       </c>
     </row>
     <row r="68" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B68" s="28" t="s">
+      <c r="B68" s="40" t="s">
         <v>89</v>
       </c>
-      <c r="C68" s="29"/>
+      <c r="C68" s="41"/>
       <c r="D68" s="7">
         <f>D65+(D66/4)</f>
-        <v>2.3406666666666665</v>
+        <v>16.387333333333334</v>
       </c>
     </row>
     <row r="71" spans="2:6" x14ac:dyDescent="0.2">
@@ -1822,25 +1868,34 @@
       </c>
     </row>
     <row r="72" spans="2:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B72" s="35" t="s">
+      <c r="B72" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="C72" s="35"/>
-      <c r="D72" s="35"/>
-      <c r="E72" s="35"/>
-      <c r="F72" s="35"/>
+      <c r="C72" s="28"/>
+      <c r="D72" s="28"/>
+      <c r="E72" s="28"/>
+      <c r="F72" s="28"/>
     </row>
     <row r="73" spans="2:6" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B73" s="35" t="s">
+      <c r="B73" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="C73" s="35"/>
-      <c r="D73" s="35"/>
-      <c r="E73" s="35"/>
-      <c r="F73" s="35"/>
+      <c r="C73" s="28"/>
+      <c r="D73" s="28"/>
+      <c r="E73" s="28"/>
+      <c r="F73" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B36:E36"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B72:F72"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="B63:C63"/>
     <mergeCell ref="B73:F73"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B37:E37"/>
@@ -1857,15 +1912,6 @@
     <mergeCell ref="B67:C67"/>
     <mergeCell ref="B66:C66"/>
     <mergeCell ref="B62:C62"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B36:E36"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B72:F72"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="B61:C61"/>
-    <mergeCell ref="B63:C63"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>